<commit_message>
Few changes done in menu and ss form
</commit_message>
<xml_diff>
--- a/files/covid-19/1/Covid19_Bulk_Import_Excel_Format.xlsx
+++ b/files/covid-19/1/Covid19_Bulk_Import_Excel_Format.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="South Sudan Import" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="sub" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="sub" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -720,39 +720,39 @@
   <dimension ref="A1:AN1003"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="W1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AC3" activeCellId="0" sqref="AC3"/>
+      <selection pane="topLeft" activeCell="AC14" activeCellId="0" sqref="AC14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="12.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="24.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="25.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="14.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="24.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="27.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="40.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="27.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="40.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="2" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="2" width="19.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="16.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="2" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="19.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="14.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="15.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="14.83"/>
@@ -14330,7 +14330,7 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="73.83"/>
@@ -14340,7 +14340,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="11" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="52.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="52.85"/>
   </cols>
   <sheetData>
     <row r="1" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>